<commit_message>
Dodano testy dla klasy TransformInverse i TransformShorten
</commit_message>
<xml_diff>
--- a/TextTransformer.xlsx
+++ b/TextTransformer.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Krzyś\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adamp\Documents\Studia\Semestr 5\Inżynieria oprogramowania\TextTransformer\Text_Transformer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16F92E33-832F-4980-B19E-1B226BE44B65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{655895CA-3A01-49DD-8F4F-B9866FBB2239}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Opis" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="74">
   <si>
     <t>Text Transformer</t>
   </si>
@@ -262,9 +262,6 @@
   </si>
   <si>
     <t>0.5</t>
-  </si>
-  <si>
-    <t>.</t>
   </si>
   <si>
     <t>Stworzenie GUI</t>
@@ -369,7 +366,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
@@ -411,8 +408,6 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -853,17 +848,17 @@
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="95.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="23.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" ht="84.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -882,16 +877,16 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="52" style="3" customWidth="1"/>
     <col min="2" max="2" width="15" style="4" customWidth="1"/>
-    <col min="3" max="3" width="21.625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="25.375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="58.125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="21.58203125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="25.33203125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="58.08203125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="18.5" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
@@ -908,7 +903,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="62" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -925,7 +920,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="108.5" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -942,7 +937,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="62" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -959,7 +954,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
@@ -976,7 +971,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>15</v>
       </c>
@@ -993,7 +988,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="93" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>17</v>
       </c>
@@ -1010,7 +1005,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>19</v>
       </c>
@@ -1027,7 +1022,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="108.5" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
@@ -1044,7 +1039,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="31" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
@@ -1061,7 +1056,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C11" s="4">
         <f>SUM(C2:C10)</f>
         <v>33</v>
@@ -1078,25 +1073,25 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A2:C45"/>
+  <dimension ref="A2:C40"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="45.125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="48.875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="45.08203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="48.83203125" style="3" customWidth="1"/>
     <col min="3" max="3" width="33" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="18.5" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
@@ -1107,7 +1102,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
         <v>28</v>
       </c>
@@ -1118,7 +1113,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6"/>
       <c r="B6" s="8" t="s">
         <v>30</v>
@@ -1127,7 +1122,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7"/>
       <c r="B7" s="8" t="s">
         <v>31</v>
@@ -1136,7 +1131,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="31" x14ac:dyDescent="0.35">
       <c r="A8"/>
       <c r="B8" s="10" t="s">
         <v>32</v>
@@ -1145,7 +1140,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9"/>
       <c r="B9" s="9" t="s">
         <v>33</v>
@@ -1154,7 +1149,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
         <v>34</v>
       </c>
@@ -1165,7 +1160,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11"/>
       <c r="B11" s="8" t="s">
         <v>36</v>
@@ -1174,7 +1169,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="31" x14ac:dyDescent="0.35">
       <c r="A12"/>
       <c r="B12" s="8" t="s">
         <v>37</v>
@@ -1183,7 +1178,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13"/>
       <c r="B13" s="9" t="s">
         <v>33</v>
@@ -1192,7 +1187,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="9" t="s">
         <v>38</v>
       </c>
@@ -1203,7 +1198,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15"/>
       <c r="B15" s="8" t="s">
         <v>40</v>
@@ -1212,7 +1207,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16"/>
       <c r="B16" s="9" t="s">
         <v>33</v>
@@ -1221,7 +1216,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="9" t="s">
         <v>41</v>
       </c>
@@ -1232,7 +1227,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18"/>
       <c r="B18" s="8" t="s">
         <v>43</v>
@@ -1241,7 +1236,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19"/>
       <c r="B19" s="9" t="s">
         <v>33</v>
@@ -1250,7 +1245,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="9" t="s">
         <v>44</v>
       </c>
@@ -1261,7 +1256,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21"/>
       <c r="B21" s="8" t="s">
         <v>46</v>
@@ -1270,7 +1265,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22"/>
       <c r="B22" s="8" t="s">
         <v>47</v>
@@ -1279,7 +1274,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23"/>
       <c r="B23" s="9" t="s">
         <v>33</v>
@@ -1288,7 +1283,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="9" t="s">
         <v>48</v>
       </c>
@@ -1299,7 +1294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="31" x14ac:dyDescent="0.35">
       <c r="A25"/>
       <c r="B25" s="8" t="s">
         <v>50</v>
@@ -1308,7 +1303,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26"/>
       <c r="B26" s="8" t="s">
         <v>51</v>
@@ -1317,7 +1312,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27"/>
       <c r="B27" s="9" t="s">
         <v>33</v>
@@ -1326,7 +1321,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" ht="31" x14ac:dyDescent="0.35">
       <c r="A28" s="9" t="s">
         <v>52</v>
       </c>
@@ -1337,7 +1332,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" ht="31" x14ac:dyDescent="0.35">
       <c r="A29"/>
       <c r="B29" s="8" t="s">
         <v>54</v>
@@ -1346,7 +1341,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30"/>
       <c r="B30" s="9" t="s">
         <v>33</v>
@@ -1355,7 +1350,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" ht="31" x14ac:dyDescent="0.35">
       <c r="A31" s="9" t="s">
         <v>55</v>
       </c>
@@ -1366,7 +1361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32"/>
       <c r="B32" s="8" t="s">
         <v>57</v>
@@ -1375,7 +1370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" ht="31" x14ac:dyDescent="0.35">
       <c r="A33"/>
       <c r="B33" s="8" t="s">
         <v>58</v>
@@ -1384,7 +1379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34"/>
       <c r="B34" s="9" t="s">
         <v>33</v>
@@ -1393,7 +1388,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="14" t="s">
         <v>59</v>
       </c>
@@ -1404,7 +1399,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B36" s="3" t="s">
         <v>61</v>
       </c>
@@ -1412,7 +1407,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B37" s="3" t="s">
         <v>64</v>
       </c>
@@ -1420,7 +1415,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B38" s="3" t="s">
         <v>62</v>
       </c>
@@ -1428,7 +1423,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B39" s="3" t="s">
         <v>63</v>
       </c>
@@ -1436,22 +1431,12 @@
         <v>65</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B40" s="9" t="s">
         <v>33</v>
       </c>
       <c r="C40" s="13">
         <v>2.5</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
-        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1467,95 +1452,95 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F0204D-81C3-4FE5-8656-6D0D0D9CF147}">
   <dimension ref="A2:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="36.875" customWidth="1"/>
+    <col min="1" max="1" width="36.83203125" customWidth="1"/>
     <col min="2" max="2" width="42" customWidth="1"/>
-    <col min="3" max="3" width="19" style="15" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="17" t="s">
+    <row r="2" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="16" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
         <v>67</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C4" s="15">
+      <c r="C5">
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
         <v>70</v>
       </c>
-      <c r="C5" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C6" s="15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B7" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="14">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
         <v>73</v>
       </c>
-      <c r="C8" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>74</v>
-      </c>
-      <c r="C9" s="15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B10" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="16">
+      <c r="C10" s="14">
         <v>3</v>
       </c>
     </row>

</xml_diff>